<commit_message>
fix : .{SheetName} should be legal fix : clear progress bar when error fix : template xlsx data error
</commit_message>
<xml_diff>
--- a/ExcelExample.xlsx
+++ b/ExcelExample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\InGitHub\greatclock\excel_to_scriptableobject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A5E1111-8532-4D65-B99F-66D93AEC9DC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B8373C-A176-45D2-B405-DBC4F3B460EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="2023" windowWidth="16457" windowHeight="9548" xr2:uid="{1132A392-AB7F-4A15-BB9A-12DA635E19A3}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13320" xr2:uid="{1132A392-AB7F-4A15-BB9A-12DA635E19A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Student" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="94">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -304,14 +304,6 @@
   </si>
   <si>
     <t>E20002</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A00001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A00002</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -855,7 +847,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>16</v>
@@ -890,7 +882,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>3</v>
@@ -925,7 +917,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>17</v>
@@ -949,7 +941,7 @@
         <v>5</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
@@ -960,7 +952,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>17</v>
@@ -995,7 +987,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>18</v>
@@ -1030,7 +1022,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>18</v>
@@ -1065,7 +1057,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>19</v>
@@ -1100,7 +1092,7 @@
         <v>10</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>19</v>
@@ -1135,7 +1127,7 @@
         <v>20</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>17</v>
@@ -1170,7 +1162,7 @@
         <v>22</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>24</v>
@@ -1205,7 +1197,7 @@
         <v>23</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>17</v>
@@ -1237,10 +1229,10 @@
         <v>19911310</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>17</v>
@@ -1279,7 +1271,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -1298,7 +1290,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>58</v>
@@ -1312,7 +1304,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>3</v>
@@ -1322,7 +1314,7 @@
       <c r="A3" s="9"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D3" s="9"/>
     </row>
@@ -1330,7 +1322,7 @@
       <c r="A4" s="9"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D4" s="9"/>
     </row>
@@ -1338,7 +1330,7 @@
       <c r="A5" s="9"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D5" s="9"/>
     </row>
@@ -1346,7 +1338,7 @@
       <c r="A6" s="9"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D6" s="9"/>
     </row>
@@ -1358,7 +1350,7 @@
         <v>59</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D7" s="9">
         <v>23450001</v>
@@ -1372,7 +1364,7 @@
         <v>60</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D8" s="9">
         <v>23450002</v>
@@ -1386,7 +1378,7 @@
         <v>61</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>63</v>
@@ -1400,7 +1392,7 @@
         <v>62</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D10" s="9">
         <v>22330002</v>
@@ -1414,7 +1406,7 @@
         <v>66</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D11" s="9">
         <v>22230001</v>
@@ -1428,7 +1420,7 @@
         <v>67</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D12" s="9">
         <v>22230002</v>
@@ -1442,7 +1434,7 @@
         <v>66</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D13" s="9">
         <v>23330001</v>
@@ -1456,7 +1448,7 @@
         <v>67</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D14" s="9">
         <v>23330002</v>
@@ -1464,13 +1456,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>72</v>
-      </c>
       <c r="C15" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D15" s="9">
         <v>22220001</v>
@@ -1478,13 +1470,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>73</v>
-      </c>
       <c r="C16" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D16" s="9">
         <v>22220002</v>
@@ -1495,10 +1487,10 @@
         <v>300001</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D17" s="9">
         <v>32220001</v>
@@ -1509,10 +1501,10 @@
         <v>300002</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D18" s="9">
         <v>32220002</v>
@@ -1520,13 +1512,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>78</v>
-      </c>
       <c r="C19" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D19" s="9">
         <v>32210001</v>
@@ -1534,13 +1526,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>79</v>
-      </c>
       <c r="C20" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D20" s="9">
         <v>32210002</v>
@@ -1551,10 +1543,10 @@
         <v>400001</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D21" s="9">
         <v>32110001</v>
@@ -1565,10 +1557,10 @@
         <v>400002</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D22" s="9">
         <v>32110002</v>
@@ -1579,10 +1571,10 @@
         <v>500001</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D23" s="9">
         <v>32100001</v>
@@ -1593,10 +1585,10 @@
         <v>500002</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D24" s="9">
         <v>32100002</v>

</xml_diff>